<commit_message>
adding tasks to ifun
</commit_message>
<xml_diff>
--- a/אפיון הפרויקט הכי חתיך😊.xlsx
+++ b/אפיון הפרויקט הכי חתיך😊.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\9090\Documents\לימודים\פרויקט גמר\Final-Project-At-React-Node-MySql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622C0024-8DDE-4EA3-950D-3479E650FC98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D83E1F-8B81-4469-B442-0E9FAA326295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="980" yWindow="2700" windowWidth="13030" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>עמוד הבית:</t>
   </si>
@@ -402,6 +402,12 @@
   </si>
   <si>
     <t>לשמור פרטי אשראי בDB?</t>
+  </si>
+  <si>
+    <t>להוסיף אפשרות של פח מהסל קניות</t>
+  </si>
+  <si>
+    <t>שאם הוא לא רוצה בסוף שיוכל להוריד את המתנה</t>
   </si>
 </sst>
 </file>
@@ -758,8 +764,8 @@
   </sheetPr>
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -840,12 +846,18 @@
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
       <c r="H10" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
+      <c r="F11" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H12" t="s">

</xml_diff>

<commit_message>
startto fix rerender of images
</commit_message>
<xml_diff>
--- a/אפיון הפרויקט הכי חתיך😊.xlsx
+++ b/אפיון הפרויקט הכי חתיך😊.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\9090\Documents\לימודים\פרויקט גמר\Final-Project-At-React-Node-MySql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C225E2B7-D6D7-40B6-B56B-331252B5255B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E5FAB3-A6CD-48A8-B482-07B69E07E35A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>עמוד הבית:</t>
   </si>
@@ -410,7 +410,10 @@
     <t>לשנות את הalt של התמוות</t>
   </si>
   <si>
-    <t>לגמור לטפל בכל ענייני התמונות</t>
+    <t>וגם צריך לפני התשלום ךבדוק שכל השדות מלאים</t>
+  </si>
+  <si>
+    <t>ואדב אחרי הקנניה את צריכה לנקות את העגלת קניות</t>
   </si>
 </sst>
 </file>
@@ -768,7 +771,7 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -868,6 +871,9 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>53</v>
+      </c>
       <c r="H13" t="s">
         <v>35</v>
       </c>

</xml_diff>